<commit_message>
Replace global MIDI read button with individual MIDI read buttons on Akai MIDIMix template.
</commit_message>
<xml_diff>
--- a/src/-/templates/i-template--keyboard+midimix.xlsx
+++ b/src/-/templates/i-template--keyboard+midimix.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="1080" windowWidth="12340" windowHeight="19380" tabRatio="500"/>
+    <workbookView xWindow="22320" yWindow="0" windowWidth="15280" windowHeight="19380" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="25">
   <si>
     <t>Pixels</t>
   </si>
@@ -49,13 +50,58 @@
   </si>
   <si>
     <t>Center Y</t>
+  </si>
+  <si>
+    <t>Knob A</t>
+  </si>
+  <si>
+    <t>Knob B</t>
+  </si>
+  <si>
+    <t>Knob C</t>
+  </si>
+  <si>
+    <t>Button A</t>
+  </si>
+  <si>
+    <t>Button B</t>
+  </si>
+  <si>
+    <t>Slider</t>
+  </si>
+  <si>
+    <t>Column 1</t>
+  </si>
+  <si>
+    <t>Column 2</t>
+  </si>
+  <si>
+    <t>Column 3</t>
+  </si>
+  <si>
+    <t>Column 4</t>
+  </si>
+  <si>
+    <t>Column 5</t>
+  </si>
+  <si>
+    <t>Column 6</t>
+  </si>
+  <si>
+    <t>Column 7</t>
+  </si>
+  <si>
+    <t>Column 8</t>
+  </si>
+  <si>
+    <t>Column 9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -87,6 +133,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -105,8 +157,206 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="283">
+  <cellStyleXfs count="481">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -394,7 +644,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="283">
+  <cellStyles count="481">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -536,6 +786,105 @@
     <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="474" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="476" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="480" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -677,6 +1026,105 @@
     <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="455" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="473" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="475" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="477" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="479" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1006,10 +1454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1020,122 +1468,508 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1">
-        <v>1100</v>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B3">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>944</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <f>(B6-(B8/2))/B2</f>
+        <v>0.82090909090909092</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>692</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <f>(B7-(B9/2))/B3</f>
+        <v>0.69058823529411761</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>82</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <f>B8/B2</f>
+        <v>7.454545454545454E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>210</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <f>B9/B3</f>
+        <v>0.24705882352941178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="B13">
+        <v>0.10272727299999999</v>
+      </c>
+      <c r="C13">
+        <f>B13+(B$12*E$8)</f>
+        <v>0.17727272754545453</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="B14">
+        <v>0.11818181799999999</v>
+      </c>
+      <c r="C14">
+        <f>B14+(B$12*E$8)</f>
+        <v>0.19272727254545452</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="B15">
+        <v>0.10272727299999999</v>
+      </c>
+      <c r="C15">
+        <f>B15+(B$12*E$8)</f>
+        <v>0.17727272754545453</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>0.10272727299999999</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <f>ROUND(B2*B19, 0)</f>
+        <v>113</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19">
+        <f>E19+(E21/2)</f>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>0.68823529400000005</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <f>ROUND(B3*B20, 0)</f>
+        <v>585</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20">
+        <f>E20+(E22/2)</f>
+        <v>695</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>7.4545454999999997E-2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <f>ROUND(B2*B21, 0)</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>0.258823529</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <f>ROUND(B3*B22, 0)</f>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>154</v>
+      </c>
+      <c r="C26">
+        <v>254</v>
+      </c>
+      <c r="D26">
+        <v>353</v>
+      </c>
+      <c r="E26">
+        <v>451</v>
+      </c>
+      <c r="F26">
+        <v>549</v>
+      </c>
+      <c r="G26">
+        <v>648</v>
+      </c>
+      <c r="H26">
+        <v>747</v>
+      </c>
+      <c r="I26">
+        <v>846</v>
+      </c>
+      <c r="J26">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="D27"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29">
+        <v>138</v>
+      </c>
+      <c r="C29">
+        <f>B29+39</f>
+        <v>177</v>
+      </c>
+      <c r="D29"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30">
+        <v>262</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:C31" si="0">B30+39</f>
+        <v>301</v>
+      </c>
+      <c r="D30"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31">
+        <v>387</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>426</v>
+      </c>
+      <c r="D31"/>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32">
+        <v>504</v>
+      </c>
+      <c r="D32"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33">
+        <v>564</v>
+      </c>
+      <c r="D33"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34">
+        <v>695</v>
+      </c>
+      <c r="D34"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection sqref="A1:J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B2">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" s="1" customFormat="1">
+        <v>154</v>
+      </c>
+      <c r="C2">
+        <v>254</v>
+      </c>
+      <c r="D2">
+        <v>353</v>
+      </c>
+      <c r="E2">
+        <v>451</v>
+      </c>
+      <c r="F2">
+        <v>549</v>
+      </c>
+      <c r="G2">
+        <v>648</v>
+      </c>
+      <c r="H2">
+        <v>747</v>
+      </c>
+      <c r="I2">
+        <v>846</v>
+      </c>
+      <c r="J2">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <f>(B5-(B7/2))/B1</f>
-        <v>-2.7272727272727271E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>138</v>
+      </c>
+      <c r="C5">
+        <f>B5+39</f>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <f>(B6-(B8/2))/B2</f>
-        <v>1.7647058823529412E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>262</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:C10" si="0">B6+39</f>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B7">
-        <v>100</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <f>B7/B1</f>
-        <v>9.0909090909090912E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>387</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B8">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <f>B8/B2</f>
-        <v>1.1764705882352941E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17">
-        <v>0.10272727299999999</v>
-      </c>
-      <c r="C17">
-        <f>B17+(B$16*E$7)</f>
-        <v>0.19363636390909089</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18">
-        <v>0.11818181799999999</v>
-      </c>
-      <c r="C18">
-        <f t="shared" ref="C18:C19" si="0">B18+(B$16*E$7)</f>
-        <v>0.20909090890909091</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="B19">
-        <v>0.10272727299999999</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
-        <v>0.19363636390909089</v>
+        <v>504</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>695</v>
       </c>
     </row>
   </sheetData>

</xml_diff>